<commit_message>
added CTD types to export_metadata
</commit_message>
<xml_diff>
--- a/devel/Type source files/Sample_types.xlsx
+++ b/devel/Type source files/Sample_types.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="79">
   <si>
     <t>AMM</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>Swim-net</t>
+  </si>
+  <si>
+    <t>Niskin bottle</t>
   </si>
 </sst>
 </file>
@@ -611,8 +614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -847,7 +850,9 @@
       <c r="B24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">

</xml_diff>

<commit_message>
Added functionality to compile species lists and check them using APIs (taxize package). Improved export_metadata
</commit_message>
<xml_diff>
--- a/devel/Type source files/Sample_types.xlsx
+++ b/devel/Type source files/Sample_types.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anette\Dropbox\Type source files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15540"/>
+    <workbookView xWindow="480" yWindow="480" windowWidth="25120" windowHeight="15040"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,18 +12,18 @@
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="120">
   <si>
     <t>AMM</t>
   </si>
@@ -405,6 +400,9 @@
   </si>
   <si>
     <t>replace with existing "sample type" i DB (CONRAD)</t>
+  </si>
+  <si>
+    <t>Ice corer 14 cm; Ice corer 9 cm; Suction pump; Slurp gun; Bottle</t>
   </si>
 </sst>
 </file>
@@ -845,7 +843,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -856,23 +854,23 @@
   <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" zoomScaleNormal="88" zoomScalePageLayoutView="88" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22:B24"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="31.28515625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" style="13" customWidth="1"/>
-    <col min="4" max="4" width="60.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" style="3"/>
+    <col min="2" max="2" width="31.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="60.33203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="11" style="3" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="19" style="3" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="124.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="3"/>
+    <col min="7" max="7" width="9.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="124.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1640625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="5" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="5" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>55</v>
       </c>
@@ -898,7 +896,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -921,7 +919,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -933,7 +931,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>4</v>
       </c>
@@ -956,7 +954,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -968,7 +966,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -980,7 +978,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -997,7 +995,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8">
       <c r="A8" s="2" t="s">
         <v>72</v>
       </c>
@@ -1011,7 +1009,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
         <v>57</v>
       </c>
@@ -1026,7 +1024,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -1041,7 +1039,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8">
       <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
@@ -1055,7 +1053,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8">
       <c r="A12" s="2" t="s">
         <v>15</v>
       </c>
@@ -1067,7 +1065,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8">
       <c r="A13" s="10" t="s">
         <v>66</v>
       </c>
@@ -1079,7 +1077,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8">
       <c r="A14" s="4" t="s">
         <v>19</v>
       </c>
@@ -1096,7 +1094,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8">
       <c r="A15" s="4" t="s">
         <v>21</v>
       </c>
@@ -1108,7 +1106,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8">
       <c r="A16" s="3" t="s">
         <v>62</v>
       </c>
@@ -1123,7 +1121,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8">
       <c r="A17" s="4" t="s">
         <v>51</v>
       </c>
@@ -1140,7 +1138,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8">
       <c r="A18" s="4" t="s">
         <v>23</v>
       </c>
@@ -1157,7 +1155,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8">
       <c r="A19" s="4" t="s">
         <v>25</v>
       </c>
@@ -1168,7 +1166,7 @@
         <v>102</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>91</v>
+        <v>119</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>82</v>
@@ -1177,7 +1175,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8">
       <c r="A20" s="4" t="s">
         <v>27</v>
       </c>
@@ -1194,7 +1192,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8">
       <c r="A21" s="3" t="s">
         <v>68</v>
       </c>
@@ -1207,7 +1205,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8">
       <c r="A22" s="3" t="s">
         <v>61</v>
       </c>
@@ -1224,7 +1222,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8">
       <c r="A23" s="4" t="s">
         <v>29</v>
       </c>
@@ -1238,7 +1236,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8">
       <c r="A24" s="4" t="s">
         <v>47</v>
       </c>
@@ -1255,7 +1253,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8">
       <c r="A25" s="2" t="s">
         <v>31</v>
       </c>
@@ -1267,7 +1265,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8">
       <c r="A26" s="4" t="s">
         <v>33</v>
       </c>
@@ -1284,7 +1282,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8">
       <c r="A27" s="4" t="s">
         <v>35</v>
       </c>
@@ -1298,7 +1296,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8">
       <c r="A28" s="4" t="s">
         <v>37</v>
       </c>
@@ -1318,7 +1316,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8">
       <c r="A29" s="2" t="s">
         <v>39</v>
       </c>
@@ -1330,7 +1328,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8">
       <c r="A30" s="4" t="s">
         <v>43</v>
       </c>
@@ -1348,7 +1346,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8">
       <c r="A31" s="4" t="s">
         <v>8</v>
       </c>
@@ -1371,7 +1369,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8">
       <c r="A32" s="4" t="s">
         <v>41</v>
       </c>
@@ -1394,7 +1392,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7">
       <c r="A33" s="2" t="s">
         <v>45</v>
       </c>
@@ -1406,7 +1404,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7">
       <c r="A34" s="4" t="s">
         <v>54</v>
       </c>
@@ -1418,7 +1416,7 @@
       </c>
       <c r="D34" s="15"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7">
       <c r="A35" s="3" t="s">
         <v>64</v>
       </c>
@@ -1430,7 +1428,7 @@
       </c>
       <c r="D35" s="17"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7">
       <c r="A36" s="4" t="s">
         <v>48</v>
       </c>
@@ -1442,7 +1440,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7">
       <c r="A37" s="4" t="s">
         <v>50</v>
       </c>
@@ -1481,62 +1479,62 @@
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="8" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1">
       <c r="A6" s="4"/>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="8" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1">
       <c r="A8" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1">
       <c r="A10" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1">
       <c r="A11" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1">
       <c r="A12" s="4" t="s">
         <v>115</v>
       </c>

</xml_diff>